<commit_message>
update api check quy cách
</commit_message>
<xml_diff>
--- a/public/excel/SapCompliance.xlsx
+++ b/public/excel/SapCompliance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TLG\DeliveryTracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soft.public\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,15 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Mã SAP</t>
   </si>
   <si>
     <t>Mã đơn vị</t>
-  </si>
-  <si>
-    <t>Mã Barcode</t>
   </si>
   <si>
     <t>KG</t>
@@ -390,23 +387,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="41" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +410,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -422,24 +418,18 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>40001374</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>5555551412</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix lỗi tạo dữ liệu excel
</commit_message>
<xml_diff>
--- a/public/excel/SapCompliance.xlsx
+++ b/public/excel/SapCompliance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soft.public\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TLG\DeliveryTracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,10 +41,10 @@
     <t>Quy cách</t>
   </si>
   <si>
-    <t>Trạng thái</t>
-  </si>
-  <si>
     <t>PSSM Tẩy Hồng 009 CYCLAMEN (XK/CR)</t>
+  </si>
+  <si>
+    <t>Check QC</t>
   </si>
 </sst>
 </file>
@@ -390,7 +390,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,7 +416,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -427,7 +427,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>20</v>

</xml_diff>